<commit_message>
xlsx: xlsxCType normalize input "s" type to internal "inlineStr"
</commit_message>
<xml_diff>
--- a/packages/jsreport-xlsx/test/xlsx/variable-replace-multi-explicit-types.xlsx
+++ b/packages/jsreport-xlsx/test/xlsx/variable-replace-multi-explicit-types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE943F5-919D-F647-8E1B-037165E4360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5094B3-5684-FC46-9401-C54C08B4AEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8760" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{BCF64815-9B49-C248-B93A-D80F9C79FAA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>{{string}}</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>{{xlsxCType t="b"}}{{boolean}}</t>
+  </si>
+  <si>
+    <t>{{xlsxCType t="s"}}{{string}}</t>
   </si>
 </sst>
 </file>
@@ -385,26 +388,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AD9493-29BA-D542-BD26-95AEB26F093C}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>